<commit_message>
Plik do Unit Testów
</commit_message>
<xml_diff>
--- a/SmallInputTest.xlsx
+++ b/SmallInputTest.xlsx
@@ -352,7 +352,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,23 +363,23 @@
       </c>
       <c r="B1">
         <f ca="1">RAND()*25</f>
-        <v>23.613339202299869</v>
+        <v>23.496284394212637</v>
       </c>
       <c r="C1">
-        <f t="shared" ref="C1:K16" ca="1" si="0">RAND()*25</f>
-        <v>4.7320829985887745</v>
+        <f t="shared" ref="C1:F10" ca="1" si="0">RAND()*25</f>
+        <v>8.1579779811291395</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2725437410265226</v>
+        <v>14.131496873973004</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3590122206068616</v>
+        <v>2.3257883351580801</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>12.555355405593716</v>
+        <v>1.5267236268714679</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -387,24 +387,24 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:K30" ca="1" si="1">RAND()*25</f>
-        <v>12.830294922339714</v>
+        <f t="shared" ref="B2:B10" ca="1" si="1">RAND()*25</f>
+        <v>7.2661776533493567</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.602547139443359</v>
+        <v>22.120297182751241</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>7.421141192195857</v>
+        <v>23.069932315115359</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1795630896224614</v>
+        <v>12.318827654064046</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3109857410931745</v>
+        <v>21.87195539249338</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -413,23 +413,23 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7033338450825135</v>
+        <v>21.204521932869131</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>21.89954088829079</v>
+        <v>21.608129763636633</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>16.398460173649955</v>
+        <v>8.1443508500372097</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>18.642357819495281</v>
+        <v>4.0499492977974141</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>11.926527184995633</v>
+        <v>11.77207886139032</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -438,23 +438,23 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>12.161730893900133</v>
+        <v>24.43176516346843</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4091566102313351</v>
+        <v>8.0519485190633837</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2024235406138297</v>
+        <v>21.260560715263253</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>18.342416648798675</v>
+        <v>0.15678458123833394</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>9.400172640044433</v>
+        <v>17.608844736419748</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -463,23 +463,23 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>14.334771293926115</v>
+        <v>7.0795835925562853</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4930508089597746</v>
+        <v>18.435392959213029</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>14.802265188349018</v>
+        <v>7.8630521186671105</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>14.078213855974983</v>
+        <v>22.180846905798905</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>19.511388251243041</v>
+        <v>8.1770705088033218</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -488,23 +488,23 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>16.485888662503946</v>
+        <v>19.677600983226846</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>17.65335809475069</v>
+        <v>20.811155540099843</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9747843171668098</v>
+        <v>17.642024242883789</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.148643412643894</v>
+        <v>7.515268550328666</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6228447885780124</v>
+        <v>22.291648438139934</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,23 +513,23 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>10.201513748926642</v>
+        <v>21.607270122763598</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8993074729720885</v>
+        <v>15.942531085691385</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8409875428638056</v>
+        <v>8.8118885484347764</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3119338306719297</v>
+        <v>22.51997778531242</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1036188100397482</v>
+        <v>2.7027162165214529</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -538,23 +538,23 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>16.838052986845284</v>
+        <v>23.157334238217636</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5829002581164469</v>
+        <v>10.90377092025801</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6937732013439124</v>
+        <v>7.2801496336517886</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1418958948333353</v>
+        <v>6.6120012404956743</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2477047737221305</v>
+        <v>3.4706206535935453</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,23 +563,23 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>24.159557393195296</v>
+        <v>10.305911787720831</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>14.215281377794364</v>
+        <v>16.531027067719688</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>18.427009861082851</v>
+        <v>9.9499805079344981</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4536694615686203</v>
+        <v>3.1514018218457061</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>19.253887216772462</v>
+        <v>12.932080667487513</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,23 +588,23 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>24.138266102290711</v>
+        <v>24.009177468095821</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3530637331604787</v>
+        <v>22.623392147731021</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>21.369409996262291</v>
+        <v>4.9916754885964894</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>15.539888279411022</v>
+        <v>21.936731912934793</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>18.236916867675209</v>
+        <v>18.46021439828213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>